<commit_message>
Upload files related to revision
</commit_message>
<xml_diff>
--- a/Source_Data/Ecoli_Replete_Labeling.xlsx
+++ b/Source_Data/Ecoli_Replete_Labeling.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardlaw/Documents/UCLA/Park Lab/ED_EMP_Glycolysis/Writing/Final/Github/Ecoli_Acetate_to_Glucose/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardlaw/Documents/UCLA/Park Lab/ED_EMP_Glycolysis/Writing/Final/Github/Source_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24B9DB2-9E74-3F4A-97C7-99007CD1E14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83507A0-D8E7-7243-8017-26FA94819423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="49200" windowHeight="28340" activeTab="2" xr2:uid="{C1AA1129-A496-174B-803F-A5F90AD6FDF7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24560" windowHeight="28300" activeTab="3" xr2:uid="{C1AA1129-A496-174B-803F-A5F90AD6FDF7}"/>
   </bookViews>
   <sheets>
     <sheet name="4a" sheetId="1" r:id="rId1"/>
     <sheet name="4b" sheetId="2" r:id="rId2"/>
     <sheet name="4c" sheetId="3" r:id="rId3"/>
+    <sheet name="Ext.5" sheetId="4" r:id="rId4"/>
+    <sheet name="Ext.10" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +31,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
   <si>
     <t>G6P M+0</t>
   </si>
@@ -210,14 +214,75 @@
   </si>
   <si>
     <t>M+5_Fragment_M+4</t>
+  </si>
+  <si>
+    <t>Time (min.)</t>
+  </si>
+  <si>
+    <t>Unlabeled</t>
+  </si>
+  <si>
+    <t>[1-D]glucose</t>
+  </si>
+  <si>
+    <t>[3-D]glucose</t>
+  </si>
+  <si>
+    <t>Average and SEM</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
+    <t>G6P</t>
+  </si>
+  <si>
+    <t>FBP</t>
+  </si>
+  <si>
+    <t>DHAP</t>
+  </si>
+  <si>
+    <t>3PG</t>
+  </si>
+  <si>
+    <t>PYR</t>
+  </si>
+  <si>
+    <t>6PG</t>
+  </si>
+  <si>
+    <t>KDPG</t>
+  </si>
+  <si>
+    <t>S7P</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>SEM</t>
+  </si>
+  <si>
+    <t>6CP</t>
+  </si>
+  <si>
+    <t>5CP</t>
+  </si>
+  <si>
+    <t>Ru5P</t>
+  </si>
+  <si>
+    <t>Turnover</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000E+00"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -250,8 +315,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -567,7 +634,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B04CE0A-D881-DA41-A6ED-ED58093B6F0D}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:D18"/>
@@ -575,379 +642,257 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
         <v>1.56311957269352E-3</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>1.3255832620294415E-3</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>6.7227852024363702E-4</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>6.1397913830510999E-3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>5.4049052994985854E-3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>6.9470671334060001E-3</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.95267235633639902</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.95218428623782281</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.94977933999463204</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>5.41388367923476E-3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>5.4615771655838743E-3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>6.3302291369849266E-3</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>3.2851113979131999E-2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>3.2485593033413675E-2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>3.5389531860558779E-2</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>8.5707195408663602E-4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>2.6063254585581962E-3</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>4.2889948550293077E-4</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>5.0266309540297402E-4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>5.3172954309335739E-4</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>4.5265386867177987E-4</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>3.1140248907604449E-4</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>2.2700962542142485E-4</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>2.6289831232661381E-4</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>4.2296621436955676E-5</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>1.2231210208264033E-5</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>2.9660048376252752E-5</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0.96069317534240162</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0.97247104740718171</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>0.97520803367471365</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>5.8346389914812353E-3</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>4.5368484209001953E-3</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>3.9651082799725505E-3</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>2.1459131079091379E-2</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>1.7875534311396917E-2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>1.8194735362290236E-2</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>1.2154416352540467E-3</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>8.3417679478165353E-4</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>4.5625320048527747E-4</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>1.0443913841258824E-2</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>4.0431522301098682E-3</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>1.8833111218353106E-3</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>0.52483888054555605</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>0.53057843730195398</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>0.52461151986371002</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>1.00290181925866E-2</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>1.227176787E-2</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>1.2512496823174599E-2</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>0.45684733995334798</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>0.45699531566073198</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>0.45526443280025197</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>8.2847613085094002E-3</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>1.5447916731436276E-4</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>7.6115505128634096E-3</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -963,315 +908,312 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
         <v>7.7482074550378879E-2</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>7.8283216467185293E-2</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>6.9988732019164807E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>6.2708234524012612E-7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>2.9553618936269591E-7</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>4.0666200229352399E-7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.92232152087059061</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.92162967091602399</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.92988031734295074</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>2.2779548082783842E-5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>4.8981429014767273E-6</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>1.2491024778137595E-5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>5.6106983821671558E-5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>2.4489425576616217E-5</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>3.5462619275567147E-5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>6.0773710760220789E-5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>2.9974239809965273E-5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>4.2960490297117178E-5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>5.6117254020525851E-5</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>2.7455272313271617E-5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>3.9629841531123461E-5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>2.4800940476372511E-2</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>2.5662568450807218E-2</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>2.0169202679367504E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>3.9571086474606148E-7</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>3.575887619277812E-7</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>2.7808347813785009E-7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0.97508249902872668</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0.9742427793016053</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>0.97974955084115223</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>1.1243865790280766E-5</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>6.5306189437176033E-6</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>5.712266238917922E-6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>3.0572991011425386E-5</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>2.5276400625183716E-5</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>2.1734569194992818E-5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>3.864316265980561E-5</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>3.2526061201211999E-5</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>2.7891530143411813E-5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>3.5704764574464622E-5</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>2.9961578055133233E-5</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>2.5630030424710748E-5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>0.45756346866509301</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>0.445460297310382</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>0.454028495977848</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>3.0649090047588663E-6</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>8.7086443878586654E-8</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>2.9846618026764809E-6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>0.54240752705800299</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>0.55453510979637399</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>0.54594323306156101</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>2.5939367898738201E-5</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>4.5058068002000016E-6</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>2.528629878871586E-5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>0.46444107088604603</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>0.44952509760240378</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>0.45518917578828055</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>2.1504585262087279E-2</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>2.5077273525757143E-2</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>2.6706225807817816E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>0.50403254759431215</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>0.51460139319133935</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>0.50757289251031934</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>1.0021796257554356E-2</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>1.0796235680499552E-2</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>1.0531705893582342E-2</v>
       </c>
     </row>
@@ -1284,7 +1226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BBFF7E-380E-894D-9539-C325D0B0A72F}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -1294,58 +1236,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="1">
         <v>0.5196571770205598</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="1">
         <v>0.50222242674502859</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="1">
         <v>0.52970124755373182</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>4.358829517025415E-2</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>4.5507368715998274E-2</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>4.2841825604324146E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>0.4281104170051227</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>0.43880779880834558</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>0.41848844565260268</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>8.6441108040634547E-3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>1.3462405730627515E-2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>8.9684811893412566E-3</v>
       </c>
     </row>
@@ -1353,13 +1295,13 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>0.29627604481767628</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>0.28194437149103807</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>0.2777103972700557</v>
       </c>
     </row>
@@ -1367,13 +1309,13 @@
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>5.4401389410478451E-2</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>5.4177930035901552E-2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>5.1319893729517327E-2</v>
       </c>
     </row>
@@ -1381,13 +1323,13 @@
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>0.40843327699078108</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>0.41326481673955928</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>0.41782344309196995</v>
       </c>
     </row>
@@ -1395,13 +1337,13 @@
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>5.1340016449553029E-2</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>5.1607396227023636E-2</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>4.9705009898127893E-2</v>
       </c>
     </row>
@@ -1409,13 +1351,13 @@
       <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>0.18954927233151117</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>0.19900548550647748</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="1">
         <v>0.20344125601032922</v>
       </c>
     </row>
@@ -1423,13 +1365,13 @@
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1437,13 +1379,13 @@
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1451,13 +1393,13 @@
       <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="3">
-        <v>0</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1465,13 +1407,13 @@
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1479,13 +1421,13 @@
       <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="3">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1493,13 +1435,13 @@
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="3">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1507,13 +1449,13 @@
       <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="1">
         <v>2.1811736129860787E-2</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="1">
         <v>0.10331309489737699</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="1">
         <v>0.14452733378506649</v>
       </c>
     </row>
@@ -1521,13 +1463,13 @@
       <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="1">
         <v>0.97818826387013913</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="1">
         <v>0.89668690510262306</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="1">
         <v>0.85547266621493345</v>
       </c>
     </row>
@@ -1535,13 +1477,13 @@
       <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="3">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1549,13 +1491,13 @@
       <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="3">
-        <v>0</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1563,13 +1505,13 @@
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="3">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3">
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1577,13 +1519,13 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="3">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1591,13 +1533,13 @@
       <c r="A22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="1">
         <v>4.007335718980734E-2</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="1">
         <v>3.7555330733826088E-2</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="1">
         <v>3.2276161082081374E-2</v>
       </c>
     </row>
@@ -1605,13 +1547,13 @@
       <c r="A23" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="1">
         <v>0.95992664281019269</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="1">
         <v>0.96244466926617389</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="1">
         <v>0.96772383891791858</v>
       </c>
     </row>
@@ -1619,13 +1561,13 @@
       <c r="A24" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="3">
-        <v>0</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1633,13 +1575,13 @@
       <c r="A25" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="3">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1647,13 +1589,13 @@
       <c r="A26" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="3">
-        <v>0</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3">
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1661,13 +1603,13 @@
       <c r="A27" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="3">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1675,13 +1617,13 @@
       <c r="A28" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="1">
         <v>0.25747135518160053</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="1">
         <v>0.21560638155686745</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="1">
         <v>0.23115755721935349</v>
       </c>
     </row>
@@ -1689,13 +1631,13 @@
       <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="1">
         <v>0.74252864481839953</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="1">
         <v>0.78439361844313249</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="1">
         <v>0.76884244278064651</v>
       </c>
     </row>
@@ -1703,13 +1645,13 @@
       <c r="A30" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="3">
-        <v>0</v>
-      </c>
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-      <c r="D30" s="3">
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1717,13 +1659,13 @@
       <c r="A31" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="3">
-        <v>0</v>
-      </c>
-      <c r="C31" s="3">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3">
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1731,13 +1673,13 @@
       <c r="A32" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="3">
-        <v>0</v>
-      </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3">
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1745,13 +1687,13 @@
       <c r="A33" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="3">
-        <v>0</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3">
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1759,13 +1701,13 @@
       <c r="A34" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="1">
         <v>4.6545068973373585E-2</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="1">
         <v>5.2120332347385473E-2</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="1">
         <v>4.7543139640231165E-2</v>
       </c>
     </row>
@@ -1773,13 +1715,13 @@
       <c r="A35" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="1">
         <v>0.95345493102662648</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="1">
         <v>0.94787966765261444</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="1">
         <v>0.95245686035976895</v>
       </c>
     </row>
@@ -1787,13 +1729,13 @@
       <c r="A36" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="3">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3">
-        <v>0</v>
-      </c>
-      <c r="D36" s="3">
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1801,13 +1743,13 @@
       <c r="A37" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="3">
-        <v>0</v>
-      </c>
-      <c r="C37" s="3">
-        <v>0</v>
-      </c>
-      <c r="D37" s="3">
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1815,13 +1757,13 @@
       <c r="A38" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="3">
-        <v>0</v>
-      </c>
-      <c r="C38" s="3">
-        <v>0</v>
-      </c>
-      <c r="D38" s="3">
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1829,13 +1771,13 @@
       <c r="A39" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="1">
         <v>1.9160625674516232E-2</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="1">
         <v>1.9532899689822018E-2</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="1">
         <v>2.0573803394740766E-2</v>
       </c>
     </row>
@@ -1843,14 +1785,666 @@
       <c r="A40" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="1">
         <v>0.98083937432548374</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="1">
         <v>0.98046710031017803</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="1">
         <v>0.9794261966052592</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F218AA6C-A29C-C44E-90E8-C85A2954D1C4}">
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>60</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+      <c r="L2">
+        <v>30</v>
+      </c>
+      <c r="M2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.8610646750275448</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.89534693847208768</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.8976758663268507</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.90441721480187276</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.96838736696610495</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.9684092374834119</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2.928738773417653E-2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.7256174010324771E-2</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.9767892826803305E-2</v>
+      </c>
+      <c r="K4" s="3">
+        <v>2.4678069303627224E-2</v>
+      </c>
+      <c r="L4" s="3">
+        <v>6.1725349242198174E-3</v>
+      </c>
+      <c r="M4" s="3">
+        <v>9.6943048110225572E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.61745061066954599</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.84928353425665704</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.91231079897671197</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.96753093786622157</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.97634812167465446</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.98298004610168055</v>
+      </c>
+      <c r="H5" s="3">
+        <v>9.0169858693394292E-2</v>
+      </c>
+      <c r="I5" s="3">
+        <v>4.0804137797100092E-2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>9.9882612681469196E-3</v>
+      </c>
+      <c r="K5" s="3">
+        <v>6.8288056419232024E-3</v>
+      </c>
+      <c r="L5" s="3">
+        <v>3.4606770069526582E-3</v>
+      </c>
+      <c r="M5" s="3">
+        <v>4.2041386894706764E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.45121706117404009</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.67572833061772819</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.73647532087137169</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.86793791731903658</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.83664240739103801</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.80299512620789226</v>
+      </c>
+      <c r="H6" s="3">
+        <v>7.3738354090021579E-2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.8016921207533496E-2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5.0340737869490122E-2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>2.6893704092831788E-2</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1.6225194034180865E-2</v>
+      </c>
+      <c r="M6" s="3">
+        <v>3.4068948385643553E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.42257222545441947</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.7196113674712068</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.70153111659382217</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.75587036677260466</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.84793359408571767</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.81733202936031135</v>
+      </c>
+      <c r="H7" s="3">
+        <v>7.0422175083757116E-2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>6.2263408793782664E-2</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3.783514963847661E-2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3.2886486678109506E-2</v>
+      </c>
+      <c r="L7" s="3">
+        <v>5.140837346135383E-2</v>
+      </c>
+      <c r="M7" s="3">
+        <v>3.9466648030747044E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.49523147993855865</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.75177474009256651</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.82421977651639045</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.87853633955384114</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.94075526303294754</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.96699713123012387</v>
+      </c>
+      <c r="H8" s="3">
+        <v>9.4880741951227129E-2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>5.1130006387093682E-2</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3.6909415229497977E-2</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1.4258028743394532E-2</v>
+      </c>
+      <c r="L8" s="3">
+        <v>6.8629183742078088E-3</v>
+      </c>
+      <c r="M8" s="3">
+        <v>8.6610727139336402E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.75952601887370241</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.93349827839972743</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.93530406751336104</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.95410534044064121</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.99084200152413082</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1.0188017955278152</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5.3154993800200383E-2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.5236409018447868E-2</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.1074221439779311E-2</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1.7819559213874816E-2</v>
+      </c>
+      <c r="L9" s="3">
+        <v>7.2565831055415768E-3</v>
+      </c>
+      <c r="M9" s="3">
+        <v>7.7854487365664428E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.74719370924590367</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.95013412533194963</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.89736114501688669</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.83741643894038253</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.98158213860122467</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1.0083154372412395</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5.7515198932202007E-2</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2.634761113535351E-2</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1.6859670502151144E-2</v>
+      </c>
+      <c r="K10" s="3">
+        <v>9.4766062611901E-2</v>
+      </c>
+      <c r="L10" s="3">
+        <v>3.5224726804804402E-2</v>
+      </c>
+      <c r="M10" s="3">
+        <v>6.4606944410977071E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.50062636504578006</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.59899874448376689</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.62014098933906669</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.66670778796215868</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.73653713286760703</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.8142184032085642</v>
+      </c>
+      <c r="H11" s="3">
+        <v>6.5672796721478258E-2</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.4175386601242362E-2</v>
+      </c>
+      <c r="J11" s="3">
+        <v>6.6917079367648138E-2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>3.8204888420963666E-2</v>
+      </c>
+      <c r="L11" s="3">
+        <v>3.944547016057267E-2</v>
+      </c>
+      <c r="M11" s="3">
+        <v>4.460230644031437E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.31999777724832795</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.60485178203825241</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.78290799750947981</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.85816299189559897</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.88766426489362527</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.91092186790378304</v>
+      </c>
+      <c r="H12" s="3">
+        <v>5.0988704261081125E-2</v>
+      </c>
+      <c r="I12" s="3">
+        <v>4.8326938467545086E-2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.9464902675757366E-2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2.3538794746200589E-2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>4.4918550274084795E-3</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1.5642595452885122E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.16074450084602368</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="3">
+        <v>6.8969298245614041E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1.3225108225108224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.45036429872495448</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="3">
+        <v>6.8081343943412906E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.29051987767584098</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1.7261904761904761</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="3">
+        <v>5.4799697656840514E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E0AB72-6BC0-EB4E-8275-1254DF8EEAD5}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.1164</v>
+      </c>
+      <c r="E3">
+        <v>8.5900000000000004E-2</v>
+      </c>
+      <c r="F3">
+        <v>9.8699999999999996E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="D4">
+        <v>3.1300000000000001E-2</v>
+      </c>
+      <c r="E4">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <v>1.9599999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>